<commit_message>
update dfc-gas-trip to use "likert" appearance
</commit_message>
<xml_diff>
--- a/survey_resources/dfc-fermata/dfc-gas-trip-v1.xlsx
+++ b/survey_resources/dfc-fermata/dfc-gas-trip-v1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="63">
   <si>
     <t>type</t>
   </si>
@@ -36,6 +36,9 @@
     <t>relevant</t>
   </si>
   <si>
+    <t>appearance</t>
+  </si>
+  <si>
     <t>start</t>
   </si>
   <si>
@@ -91,6 +94,9 @@
   </si>
   <si>
     <t>Please indicate the extent to which you agree or disagree.</t>
+  </si>
+  <si>
+    <t>likert</t>
   </si>
   <si>
     <t>list_name</t>
@@ -530,13 +536,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -555,89 +561,95 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" t="s">
         <v>12</v>
       </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" t="s">
-        <v>11</v>
-      </c>
       <c r="F5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E7" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="G7" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -655,7 +667,7 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -664,62 +676,62 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C4" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B5" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C5" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B6" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C6" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -727,13 +739,13 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C7" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D7">
         <v>2</v>
@@ -741,13 +753,13 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B8" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C8" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D8">
         <v>3</v>
@@ -755,13 +767,13 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B9" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C9" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D9">
         <v>4</v>
@@ -769,13 +781,13 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B10" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C10" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D10">
         <v>5</v>
@@ -783,13 +795,13 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B11" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C11" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D11">
         <v>7</v>
@@ -797,13 +809,13 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B12" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C12" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D12">
         <v>8</v>
@@ -811,57 +823,57 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B13" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C13" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B14" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C14" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B15" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C15" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B16" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C16" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B17" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C17" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>